<commit_message>
Updated Inventory with new Mg and Zn
</commit_message>
<xml_diff>
--- a/Charge 11 - T09.xlsx
+++ b/Charge 11 - T09.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10410" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10410" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Elements Data" sheetId="4" r:id="rId1"/>
@@ -1146,7 +1146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1537,6 +1537,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5436,7 +5437,7 @@
   </sheetPr>
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
@@ -8402,9 +8403,9 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -8439,7 +8440,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="166">
-        <v>4.6310000000000002</v>
+        <v>4.5330000000000004</v>
       </c>
       <c r="B2" s="125">
         <v>0</v>
@@ -8462,7 +8463,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="166">
-        <v>6.4029999999999996</v>
+        <v>5.0609999999999999</v>
       </c>
       <c r="B3" s="125">
         <v>0</v>
@@ -8482,7 +8483,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="166">
-        <v>7.2080000000000002</v>
+        <v>5.6879999999999997</v>
       </c>
       <c r="B4" s="125">
         <v>0</v>
@@ -8502,7 +8503,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="166">
-        <v>8.0250000000000004</v>
+        <v>6.0830000000000002</v>
       </c>
       <c r="B5" s="125">
         <v>0</v>
@@ -8514,7 +8515,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="166">
-        <v>8.6</v>
+        <v>6.2190000000000003</v>
       </c>
       <c r="B6" s="125">
         <v>0</v>
@@ -8523,10 +8524,11 @@
         <f>IF(A6=0, 0, A6*B6)</f>
         <v>0</v>
       </c>
+      <c r="E6" s="189"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="166">
-        <v>8.827</v>
+        <v>6.2510000000000003</v>
       </c>
       <c r="B7" s="125">
         <v>0</v>
@@ -8537,7 +8539,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="166"/>
+      <c r="A8" s="166">
+        <v>6.2910000000000004</v>
+      </c>
       <c r="B8" s="125">
         <v>0</v>
       </c>
@@ -8547,7 +8551,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="166"/>
+      <c r="A9" s="166">
+        <v>6.7640000000000002</v>
+      </c>
       <c r="B9" s="125">
         <v>0</v>
       </c>
@@ -8557,7 +8563,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="166"/>
+      <c r="A10" s="166">
+        <v>6.9279999999999999</v>
+      </c>
       <c r="B10" s="125">
         <v>0</v>
       </c>
@@ -8567,7 +8575,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="166"/>
+      <c r="A11" s="166">
+        <v>7.1589999999999998</v>
+      </c>
       <c r="B11" s="125">
         <v>0</v>
       </c>
@@ -8577,7 +8587,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="166"/>
+      <c r="A12" s="166">
+        <v>7.1779999999999999</v>
+      </c>
       <c r="B12" s="125">
         <v>0</v>
       </c>
@@ -8587,7 +8599,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="166"/>
+      <c r="A13" s="166">
+        <v>7.2329999999999997</v>
+      </c>
       <c r="B13" s="125">
         <v>0</v>
       </c>
@@ -8597,7 +8611,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="166"/>
+      <c r="A14" s="166">
+        <v>7.3159999999999998</v>
+      </c>
       <c r="B14" s="125">
         <v>0</v>
       </c>
@@ -8607,7 +8623,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="166"/>
+      <c r="A15" s="166">
+        <v>7.992</v>
+      </c>
       <c r="B15" s="125">
         <v>0</v>
       </c>
@@ -8617,7 +8635,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="166"/>
+      <c r="A16" s="166">
+        <v>7.9960000000000004</v>
+      </c>
       <c r="B16" s="125">
         <v>0</v>
       </c>
@@ -8627,7 +8647,9 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="166"/>
+      <c r="A17" s="166">
+        <v>8.5570000000000004</v>
+      </c>
       <c r="B17" s="125">
         <v>0</v>
       </c>
@@ -8637,7 +8659,9 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="166"/>
+      <c r="A18" s="166">
+        <v>8.5619999999999994</v>
+      </c>
       <c r="B18" s="125">
         <v>0</v>
       </c>
@@ -8647,7 +8671,9 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="166"/>
+      <c r="A19" s="166">
+        <v>8.7479999999999993</v>
+      </c>
       <c r="B19" s="125">
         <v>0</v>
       </c>
@@ -8657,7 +8683,9 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="166"/>
+      <c r="A20" s="166">
+        <v>9.2379999999999995</v>
+      </c>
       <c r="B20" s="125">
         <v>0</v>
       </c>
@@ -8667,7 +8695,9 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="166"/>
+      <c r="A21" s="166">
+        <v>10.473000000000001</v>
+      </c>
       <c r="B21" s="125">
         <v>0</v>
       </c>
@@ -8677,7 +8707,9 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="166"/>
+      <c r="A22" s="166">
+        <v>10.641999999999999</v>
+      </c>
       <c r="B22" s="125">
         <v>0</v>
       </c>
@@ -8687,7 +8719,9 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="166"/>
+      <c r="A23" s="166">
+        <v>10.866</v>
+      </c>
       <c r="B23" s="125">
         <v>0</v>
       </c>
@@ -8697,7 +8731,9 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="166"/>
+      <c r="A24" s="166">
+        <v>11.372999999999999</v>
+      </c>
       <c r="B24" s="125">
         <v>0</v>
       </c>
@@ -8996,7 +9032,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -9031,7 +9067,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="125">
-        <v>7.9569999999999999</v>
+        <v>7.9279999999999999</v>
       </c>
       <c r="B2" s="125">
         <v>0</v>
@@ -9054,7 +9090,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="125">
-        <v>9.8140000000000001</v>
+        <v>9.782</v>
       </c>
       <c r="B3" s="125">
         <v>0</v>
@@ -9073,7 +9109,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="125">
-        <v>10.753</v>
+        <v>10.72</v>
       </c>
       <c r="B4" s="125">
         <v>0</v>
@@ -9092,7 +9128,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="125">
-        <v>11.766</v>
+        <v>11.714</v>
       </c>
       <c r="B5" s="125">
         <v>0</v>
@@ -9104,7 +9140,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="125">
-        <v>12.38</v>
+        <v>12.263</v>
       </c>
       <c r="B6" s="125">
         <v>0</v>
@@ -9116,7 +9152,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="125">
-        <v>12.622</v>
+        <v>12.552</v>
       </c>
       <c r="B7" s="125">
         <v>0</v>
@@ -9128,7 +9164,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="125">
-        <v>12.919</v>
+        <v>12.731</v>
       </c>
       <c r="B8" s="125">
         <v>0</v>
@@ -9140,7 +9176,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="125">
-        <v>13.013999999999999</v>
+        <v>12.920999999999999</v>
       </c>
       <c r="B9" s="125">
         <v>0</v>
@@ -9152,7 +9188,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="125">
-        <v>13.234</v>
+        <v>13.132</v>
       </c>
       <c r="B10" s="125">
         <v>0</v>
@@ -9164,7 +9200,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="125">
-        <v>14.38</v>
+        <v>14.324999999999999</v>
       </c>
       <c r="B11" s="125">
         <v>0</v>
@@ -9176,7 +9212,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="125">
-        <v>14.795999999999999</v>
+        <v>14.746</v>
       </c>
       <c r="B12" s="125">
         <v>0</v>
@@ -9188,7 +9224,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="125">
-        <v>15.32</v>
+        <v>15.217000000000001</v>
       </c>
       <c r="B13" s="125">
         <v>0</v>
@@ -9200,7 +9236,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="125">
-        <v>16.3</v>
+        <v>16.824999999999999</v>
       </c>
       <c r="B14" s="125">
         <v>0</v>
@@ -9212,7 +9248,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="125">
-        <v>17.824000000000002</v>
+        <v>17.745999999999999</v>
       </c>
       <c r="B15" s="125">
         <v>0</v>
@@ -9224,7 +9260,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="125">
-        <v>19.215</v>
+        <v>19.149000000000001</v>
       </c>
       <c r="B16" s="125">
         <v>0</v>
@@ -9236,7 +9272,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="125">
-        <v>19.731999999999999</v>
+        <v>19.539000000000001</v>
       </c>
       <c r="B17" s="125">
         <v>0</v>
@@ -9248,7 +9284,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="125">
-        <v>19.754000000000001</v>
+        <v>19.594999999999999</v>
       </c>
       <c r="B18" s="125">
         <v>0</v>
@@ -9260,7 +9296,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="125">
-        <v>19.841999999999999</v>
+        <v>19.702000000000002</v>
       </c>
       <c r="B19" s="125">
         <v>0</v>
@@ -9272,7 +9308,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="125">
-        <v>20.332000000000001</v>
+        <v>19.864999999999998</v>
       </c>
       <c r="B20" s="125">
         <v>0</v>
@@ -9284,7 +9320,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="125">
-        <v>20.411999999999999</v>
+        <v>20.327999999999999</v>
       </c>
       <c r="B21" s="125">
         <v>0</v>
@@ -9296,7 +9332,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="125">
-        <v>20.777000000000001</v>
+        <v>20.693000000000001</v>
       </c>
       <c r="B22" s="125">
         <v>0</v>
@@ -9308,7 +9344,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="125">
-        <v>21.151</v>
+        <v>21.050999999999998</v>
       </c>
       <c r="B23" s="125">
         <v>0</v>
@@ -9320,7 +9356,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="125">
-        <v>21.282</v>
+        <v>21.161999999999999</v>
       </c>
       <c r="B24" s="125">
         <v>0</v>

</xml_diff>